<commit_message>
Upload file first commit
</commit_message>
<xml_diff>
--- a/Pagos Eventuales realizados/08- AGOSTO/02- 29.8.23/Agentes a pagar - 29.8.23.xlsx
+++ b/Pagos Eventuales realizados/08- AGOSTO/02- 29.8.23/Agentes a pagar - 29.8.23.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$J$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$J$59</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Nro control</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>EX-1042-0034-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARTINEZ IRIS MARIANELA  </t>
+  </si>
+  <si>
+    <t>EX-2023-02283961- -GDESDE-CGE</t>
   </si>
 </sst>
 </file>
@@ -326,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -391,11 +397,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -440,12 +459,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -467,281 +480,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1202,11 +952,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,7 +970,7 @@
     <col min="7" max="7" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.33203125" customWidth="1"/>
     <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1230,7 +980,7 @@
       <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1251,37 +1001,37 @@
       <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="30" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="28">
+      <c r="A2" s="35">
         <v>2020</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="28">
         <v>2020</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30">
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="28">
         <v>2020</v>
       </c>
     </row>
@@ -1290,14 +1040,14 @@
         <v>30</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="34"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="19"/>
       <c r="I4" s="12"/>
-      <c r="J4" s="30">
+      <c r="J4" s="28">
         <v>2020</v>
       </c>
     </row>
@@ -1317,7 +1067,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="21"/>
-      <c r="J5" s="31">
+      <c r="J5" s="29">
         <v>2020</v>
       </c>
     </row>
@@ -1327,7 +1077,7 @@
         <f>F6/#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="6"/>
       <c r="E6" s="8"/>
       <c r="F6" s="14">
@@ -1337,7 +1087,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="30">
+      <c r="J6" s="28">
         <v>2020</v>
       </c>
     </row>
@@ -1345,9 +1095,9 @@
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="32"/>
       <c r="H7" s="19"/>
-      <c r="J7" s="30">
+      <c r="J7" s="28">
         <v>2020</v>
       </c>
     </row>
@@ -1367,7 +1117,7 @@
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="31">
+      <c r="J8" s="29">
         <v>2020</v>
       </c>
     </row>
@@ -1376,7 +1126,7 @@
       <c r="B9" s="13">
         <v>0</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="6"/>
       <c r="E9" s="8"/>
       <c r="F9" s="14">
@@ -1386,37 +1136,37 @@
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="30">
+      <c r="J9" s="28">
         <v>2020</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="28">
+      <c r="A10" s="35">
         <v>2021</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30">
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="28">
         <v>2021</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1425,14 +1175,14 @@
         <v>36</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="34"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="19"/>
       <c r="I12" s="12"/>
-      <c r="J12" s="30">
+      <c r="J12" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1452,7 +1202,7 @@
       </c>
       <c r="H13" s="25"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="31">
+      <c r="J13" s="29">
         <v>2021</v>
       </c>
     </row>
@@ -1461,7 +1211,7 @@
       <c r="B14" s="13">
         <v>0</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
       <c r="F14" s="14">
@@ -1471,7 +1221,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="30">
+      <c r="J14" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1480,14 +1230,14 @@
         <v>39</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="34"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="19"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="30">
+      <c r="J15" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1507,7 +1257,7 @@
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="31">
+      <c r="J16" s="29">
         <v>2021</v>
       </c>
     </row>
@@ -1516,7 +1266,7 @@
       <c r="B17" s="13">
         <v>0</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
       <c r="F17" s="14">
@@ -1526,7 +1276,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="30">
+      <c r="J17" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1535,14 +1285,14 @@
         <v>42</v>
       </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="34"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="19"/>
       <c r="I18" s="12"/>
-      <c r="J18" s="30">
+      <c r="J18" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1562,7 +1312,7 @@
       </c>
       <c r="H19" s="25"/>
       <c r="I19" s="21"/>
-      <c r="J19" s="31">
+      <c r="J19" s="29">
         <v>2021</v>
       </c>
     </row>
@@ -1571,7 +1321,7 @@
       <c r="B20" s="13">
         <v>0</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8"/>
       <c r="F20" s="14">
@@ -1581,7 +1331,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="30">
+      <c r="J20" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1590,14 +1340,14 @@
         <v>23</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="34"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="19"/>
       <c r="I21" s="12"/>
-      <c r="J21" s="30">
+      <c r="J21" s="28">
         <v>2021</v>
       </c>
     </row>
@@ -1617,7 +1367,7 @@
       </c>
       <c r="H22" s="25"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="31">
+      <c r="J22" s="29">
         <v>2021</v>
       </c>
     </row>
@@ -1626,7 +1376,7 @@
       <c r="B23" s="13">
         <v>0</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8"/>
       <c r="F23" s="14">
@@ -1636,37 +1386,37 @@
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="30">
+      <c r="J23" s="28">
         <v>2021</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="28">
-        <v>2022</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="30">
+      <c r="A24" s="35">
+        <v>2022</v>
+      </c>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="28">
         <v>2022</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="30">
+      <c r="A25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="28">
         <v>2022</v>
       </c>
     </row>
@@ -1675,14 +1425,14 @@
         <v>19</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="34"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="19"/>
       <c r="I26" s="12"/>
-      <c r="J26" s="30">
+      <c r="J26" s="28">
         <v>2022</v>
       </c>
     </row>
@@ -1712,7 +1462,7 @@
         <v>68</v>
       </c>
       <c r="I27" s="21"/>
-      <c r="J27" s="31">
+      <c r="J27" s="29">
         <v>2022</v>
       </c>
     </row>
@@ -1722,7 +1472,7 @@
         <f>F28/F27</f>
         <v>1</v>
       </c>
-      <c r="C28" s="36"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8"/>
       <c r="F28" s="14">
@@ -1732,7 +1482,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="8"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="30">
+      <c r="J28" s="28">
         <v>2022</v>
       </c>
     </row>
@@ -1741,14 +1491,14 @@
         <v>17</v>
       </c>
       <c r="B29" s="12"/>
-      <c r="C29" s="34"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="19"/>
       <c r="I29" s="12"/>
-      <c r="J29" s="30">
+      <c r="J29" s="28">
         <v>2022</v>
       </c>
     </row>
@@ -1778,7 +1528,7 @@
         <v>68</v>
       </c>
       <c r="I30" s="21"/>
-      <c r="J30" s="31">
+      <c r="J30" s="29">
         <v>2022</v>
       </c>
     </row>
@@ -1788,7 +1538,7 @@
         <f>F31/F30</f>
         <v>1</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8"/>
       <c r="F31" s="14">
@@ -1798,7 +1548,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="8"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="30">
+      <c r="J31" s="28">
         <v>2022</v>
       </c>
     </row>
@@ -1814,7 +1564,7 @@
       <c r="G32"/>
       <c r="H32" s="16"/>
       <c r="I32"/>
-      <c r="J32" s="30">
+      <c r="J32" s="28">
         <v>2022</v>
       </c>
     </row>
@@ -1844,7 +1594,7 @@
         <v>59</v>
       </c>
       <c r="I33" s="21"/>
-      <c r="J33" s="31">
+      <c r="J33" s="29">
         <v>2022</v>
       </c>
     </row>
@@ -1874,7 +1624,7 @@
         <v>61</v>
       </c>
       <c r="I34" s="21"/>
-      <c r="J34" s="31">
+      <c r="J34" s="29">
         <v>2022</v>
       </c>
     </row>
@@ -1904,7 +1654,7 @@
         <v>60</v>
       </c>
       <c r="I35" s="21"/>
-      <c r="J35" s="31">
+      <c r="J35" s="29">
         <v>2022</v>
       </c>
     </row>
@@ -1934,7 +1684,7 @@
         <v>72</v>
       </c>
       <c r="I36" s="21"/>
-      <c r="J36" s="31">
+      <c r="J36" s="29">
         <v>2022</v>
       </c>
     </row>
@@ -1963,89 +1713,89 @@
       <c r="H37" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="31">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="B38" s="13">
-        <f>F38/F37</f>
-        <v>5</v>
-      </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="14">
-        <f>SUBTOTAL(9,F33:F37)</f>
-        <v>300000</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="30">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="I37" s="37"/>
+      <c r="J37" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="24">
+        <v>23048819</v>
+      </c>
+      <c r="D38" s="5">
+        <v>39285621</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="9">
+        <v>60000</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="37"/>
+      <c r="J38" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="13">
+        <f>F39/F37</f>
+        <v>6</v>
+      </c>
+      <c r="C39" s="33"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="14">
+        <f>SUM(F33:F38)</f>
+        <v>360000</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="28">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="30">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="24">
-        <v>38780972</v>
-      </c>
-      <c r="D40" s="5">
-        <v>62006941</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="5">
-        <v>80000</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="31">
+      <c r="B40" s="20"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="28">
         <v>2022</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="24">
-        <v>40287663</v>
+        <v>38780972</v>
       </c>
       <c r="D41" s="5">
-        <v>29053244</v>
+        <v>62006941</v>
       </c>
       <c r="E41" s="25" t="s">
         <v>10</v>
@@ -2057,86 +1807,86 @@
         <v>9</v>
       </c>
       <c r="H41" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I41" s="21"/>
+      <c r="J41" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="24">
+        <v>40287663</v>
+      </c>
+      <c r="D42" s="5">
+        <v>29053244</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="5">
+        <v>80000</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="31">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B42" s="13">
-        <f>F42/F41</f>
+      <c r="I42" s="21"/>
+      <c r="J42" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="13">
+        <f>F43/F42</f>
         <v>2</v>
       </c>
-      <c r="D42" s="18"/>
-      <c r="F42" s="14">
-        <f>SUBTOTAL(9,F40:F41)</f>
+      <c r="D43" s="18"/>
+      <c r="F43" s="14">
+        <f>SUBTOTAL(9,F41:F42)</f>
         <v>160000</v>
       </c>
-      <c r="H42" s="16"/>
-      <c r="J42" s="30">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="H43" s="16"/>
+      <c r="J43" s="28">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="30">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="B44" s="20"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="28">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="24">
-        <v>38780972</v>
-      </c>
-      <c r="D44" s="5">
-        <v>62006941</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="5">
-        <v>60000</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="31">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="26">
-        <v>29053244</v>
+      <c r="C45" s="24">
+        <v>38780972</v>
+      </c>
+      <c r="D45" s="5">
+        <v>62006941</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>11</v>
@@ -2148,25 +1898,25 @@
         <v>29</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I45" s="21"/>
-      <c r="J45" s="31">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>58</v>
+      <c r="J45" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="24">
-        <v>43793838</v>
-      </c>
-      <c r="D46" s="5">
-        <v>90077722</v>
+      <c r="C46" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="26">
+        <v>29053244</v>
       </c>
       <c r="E46" s="25" t="s">
         <v>11</v>
@@ -2178,25 +1928,25 @@
         <v>29</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I46" s="21"/>
-      <c r="J46" s="31">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C47" s="24">
-        <v>23687924</v>
+        <v>43793838</v>
       </c>
       <c r="D47" s="5">
-        <v>39315002</v>
+        <v>90077722</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>11</v>
@@ -2207,25 +1957,26 @@
       <c r="G47" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H47" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J47" s="31">
+      <c r="H47" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I47" s="21"/>
+      <c r="J47" s="29">
         <v>2022</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C48" s="24">
-        <v>28458538</v>
+        <v>23687924</v>
       </c>
       <c r="D48" s="5">
-        <v>58301914</v>
+        <v>39315002</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>11</v>
@@ -2237,114 +1988,113 @@
         <v>29</v>
       </c>
       <c r="H48" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J48" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="24">
+        <v>28458538</v>
+      </c>
+      <c r="D49" s="5">
+        <v>58301914</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="5">
+        <v>60000</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J48" s="31">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="13">
-        <f>F49/F48</f>
+      <c r="J49" s="29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B50" s="13">
+        <f>F50/F49</f>
         <v>5</v>
       </c>
-      <c r="F49" s="14">
-        <f>SUBTOTAL(9,F44:F48)</f>
+      <c r="F50" s="14">
+        <f>SUBTOTAL(9,F45:F49)</f>
         <v>300000</v>
       </c>
-      <c r="H49" s="16"/>
-      <c r="J49" s="30">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="28">
+      <c r="H50" s="16"/>
+      <c r="J50" s="28">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="35">
         <v>2023</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="30">
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="28">
         <v>2023</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="30">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="35"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="28">
         <v>2023</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="30">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" s="24">
-        <v>29123698</v>
-      </c>
-      <c r="D53" s="5">
-        <v>90073435</v>
-      </c>
-      <c r="E53" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F53" s="5">
-        <v>75000</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="31">
+      <c r="B53" s="20"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="28">
         <v>2023</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C54" s="24">
-        <v>40603835</v>
+        <v>29123698</v>
       </c>
       <c r="D54" s="5">
-        <v>90073333</v>
+        <v>90073435</v>
       </c>
       <c r="E54" s="25" t="s">
         <v>27</v>
@@ -2355,139 +2105,169 @@
       <c r="G54" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H54" s="25" t="s">
+      <c r="H54" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I54" s="21"/>
+      <c r="J54" s="29">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="24">
+        <v>40603835</v>
+      </c>
+      <c r="D55" s="5">
+        <v>90073333</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="5">
+        <v>75000</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H55" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="I54" s="21"/>
-      <c r="J54" s="31">
+      <c r="I55" s="21"/>
+      <c r="J55" s="29">
         <v>2023</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="13">
-        <f>F55/F53</f>
+    <row r="56" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="12"/>
+      <c r="B56" s="13">
+        <f>F56/F54</f>
         <v>2</v>
       </c>
-      <c r="C55" s="34"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="14">
-        <f>SUBTOTAL(9,F53:F54)</f>
+      <c r="C56" s="32"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="14">
+        <f>SUBTOTAL(9,F54:F55)</f>
         <v>150000</v>
       </c>
-      <c r="G55" s="12"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="30">
+      <c r="G56" s="12"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="28">
         <v>2023</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="30">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="24">
-        <v>29123698</v>
-      </c>
-      <c r="D57" s="5">
-        <v>90073435</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F57" s="5">
-        <v>75000</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="I57" s="21"/>
-      <c r="J57" s="31">
+      <c r="B57" s="20"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="28">
         <v>2023</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C58" s="24">
-        <v>40603835</v>
+        <v>29123698</v>
       </c>
       <c r="D58" s="5">
-        <v>90073333</v>
+        <v>90073435</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F58" s="5">
         <v>75000</v>
       </c>
       <c r="G58" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I58" s="21"/>
+      <c r="J58" s="29">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="24">
+        <v>40603835</v>
+      </c>
+      <c r="D59" s="5">
+        <v>90073333</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" s="5">
+        <v>75000</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H58" s="25" t="s">
+      <c r="H59" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="I58" s="21"/>
-      <c r="J58" s="31">
+      <c r="I59" s="21"/>
+      <c r="J59" s="29">
         <v>2023</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="13">
-        <f>F59/F58</f>
+    <row r="60" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="12"/>
+      <c r="B60" s="13">
+        <f>F60/F59</f>
         <v>2</v>
       </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="14">
-        <f>SUBTOTAL(9,F57:F58)</f>
+      <c r="C60" s="32"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="14">
+        <f>SUBTOTAL(9,F58:F59)</f>
         <v>150000</v>
       </c>
-      <c r="G59" s="12"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="31">
+      <c r="G60" s="12"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="29">
         <v>2023</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J58"/>
+  <autoFilter ref="A1:J59"/>
   <mergeCells count="4">
     <mergeCell ref="A24:I25"/>
     <mergeCell ref="A10:I11"/>
     <mergeCell ref="A2:I3"/>
-    <mergeCell ref="A50:I51"/>
+    <mergeCell ref="A51:I52"/>
   </mergeCells>
-  <conditionalFormatting sqref="H38:H39 H41:H43 H45 H47 H49:H53 H1:H34 H55:H57 H59:H1048576">
+  <conditionalFormatting sqref="H39:H40 H42:H44 H46 H48 H50:H54 H1:H34 H56:H58 H60:H1048576">
     <cfRule type="duplicateValues" dxfId="15" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
@@ -2496,40 +2276,40 @@
   <conditionalFormatting sqref="H36">
     <cfRule type="duplicateValues" dxfId="13" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
+  <conditionalFormatting sqref="H37:H38">
     <cfRule type="duplicateValues" dxfId="12" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
+  <conditionalFormatting sqref="H41">
     <cfRule type="duplicateValues" dxfId="11" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
+  <conditionalFormatting sqref="H45">
     <cfRule type="duplicateValues" dxfId="10" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
+  <conditionalFormatting sqref="H47">
     <cfRule type="duplicateValues" dxfId="9" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
+  <conditionalFormatting sqref="H49">
     <cfRule type="duplicateValues" dxfId="8" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55:H57 H1:H53 H59:H1048576">
+  <conditionalFormatting sqref="H56:H58 H1:H54 H60:H1048576">
     <cfRule type="duplicateValues" dxfId="7" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H53">
+  <conditionalFormatting sqref="H54">
     <cfRule type="duplicateValues" dxfId="6" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
+  <conditionalFormatting sqref="H58">
     <cfRule type="duplicateValues" dxfId="5" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H54">
+  <conditionalFormatting sqref="H55">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H54">
+  <conditionalFormatting sqref="H55">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H58">
+  <conditionalFormatting sqref="H59">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H58">
+  <conditionalFormatting sqref="H59">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">

</xml_diff>